<commit_message>
cleaning up: better comments, automatic plate IDs, plotting by compound instead of plate so now it's possible to divide measurements across plates
</commit_message>
<xml_diff>
--- a/JWS CTG plater import template.xlsx
+++ b/JWS CTG plater import template.xlsx
@@ -6,10 +6,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevenson/Documents/git/plateplotr/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevenson/Library/CloudStorage/Box-Box/Shokat/bio lab notebook/JS-B2-79 CTG K562 DasatiLink PonatiLink/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB13A0A7-6C1F-3542-8A75-C7AD1DCD8496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B9E927-EDF7-AA41-9AB3-C8E09F772BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{2712D622-CD40-B842-AED5-08F459FD295F}"/>
   </bookViews>
@@ -99,7 +99,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -130,6 +130,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -149,7 +156,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -187,22 +194,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
+    <cellStyle name="Linked Cell" xfId="4" builtinId="24"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
@@ -519,7 +538,7 @@
   <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,11 +587,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="3" t="str">
@@ -620,7 +639,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1958,14 +1977,14 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B31">
         <f>B$1</f>
         <v>1</v>
       </c>
       <c r="C31">
-        <f t="shared" ref="C31:L31" si="15">C$1</f>
+        <f t="shared" ref="C31:L41" si="15">C$1</f>
         <v>2</v>
       </c>
       <c r="D31">
@@ -2011,7 +2030,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
-        <f t="shared" ref="A32:A39" si="16">A52</f>
+        <f>A12</f>
         <v>A</v>
       </c>
       <c r="B32" s="3" t="str">
@@ -2019,414 +2038,294 @@
         <v>NA</v>
       </c>
       <c r="C32" s="3" t="str">
-        <f t="shared" ref="B32:M39" si="17">$B$2</f>
+        <f t="shared" ref="B32:M39" si="16">$B$2</f>
         <v>NA</v>
       </c>
       <c r="D32" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="E32" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="F32" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="G32" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="H32" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="I32" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="J32" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="K32" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="L32" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="M32" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
-        <f t="shared" si="16"/>
+        <f>A13</f>
         <v>B</v>
       </c>
       <c r="B33" s="3" t="str">
-        <f t="shared" si="17"/>
-        <v>NA</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="F33">
-        <v>1</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-      <c r="I33">
-        <v>1</v>
-      </c>
-      <c r="J33">
-        <v>1</v>
-      </c>
-      <c r="K33">
-        <v>1</v>
-      </c>
-      <c r="L33">
-        <v>1</v>
-      </c>
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
       <c r="M33" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
-        <f t="shared" si="16"/>
+        <f>A14</f>
         <v>C</v>
       </c>
       <c r="B34" s="3" t="str">
-        <f t="shared" si="17"/>
-        <v>NA</v>
-      </c>
-      <c r="C34">
-        <v>2</v>
-      </c>
-      <c r="D34">
-        <v>2</v>
-      </c>
-      <c r="E34">
-        <v>2</v>
-      </c>
-      <c r="F34">
-        <v>2</v>
-      </c>
-      <c r="G34">
-        <v>2</v>
-      </c>
-      <c r="H34">
-        <v>2</v>
-      </c>
-      <c r="I34">
-        <v>2</v>
-      </c>
-      <c r="J34">
-        <v>2</v>
-      </c>
-      <c r="K34">
-        <v>2</v>
-      </c>
-      <c r="L34">
-        <v>2</v>
-      </c>
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
       <c r="M34" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
-        <f t="shared" si="16"/>
+        <f>A15</f>
         <v>D</v>
       </c>
       <c r="B35" s="3" t="str">
-        <f t="shared" si="17"/>
-        <v>NA</v>
-      </c>
-      <c r="C35">
-        <v>3</v>
-      </c>
-      <c r="D35">
-        <v>3</v>
-      </c>
-      <c r="E35">
-        <v>3</v>
-      </c>
-      <c r="F35">
-        <v>3</v>
-      </c>
-      <c r="G35">
-        <v>3</v>
-      </c>
-      <c r="H35">
-        <v>3</v>
-      </c>
-      <c r="I35">
-        <v>3</v>
-      </c>
-      <c r="J35">
-        <v>3</v>
-      </c>
-      <c r="K35">
-        <v>3</v>
-      </c>
-      <c r="L35">
-        <v>3</v>
-      </c>
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
       <c r="M35" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
-        <f t="shared" si="16"/>
+        <f>A16</f>
         <v>E</v>
       </c>
       <c r="B36" s="3" t="str">
-        <f t="shared" si="17"/>
-        <v>NA</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-      <c r="I36">
-        <v>1</v>
-      </c>
-      <c r="J36">
-        <v>1</v>
-      </c>
-      <c r="K36">
-        <v>1</v>
-      </c>
-      <c r="L36">
-        <v>1</v>
-      </c>
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
       <c r="M36" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
-        <f t="shared" si="16"/>
+        <f>A17</f>
         <v>F</v>
       </c>
       <c r="B37" s="3" t="str">
-        <f t="shared" si="17"/>
-        <v>NA</v>
-      </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="D37">
-        <v>2</v>
-      </c>
-      <c r="E37">
-        <v>2</v>
-      </c>
-      <c r="F37">
-        <v>2</v>
-      </c>
-      <c r="G37">
-        <v>2</v>
-      </c>
-      <c r="H37">
-        <v>2</v>
-      </c>
-      <c r="I37">
-        <v>2</v>
-      </c>
-      <c r="J37">
-        <v>2</v>
-      </c>
-      <c r="K37">
-        <v>2</v>
-      </c>
-      <c r="L37">
-        <v>2</v>
-      </c>
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
       <c r="M37" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
-        <f t="shared" si="16"/>
+        <f>A18</f>
         <v>G</v>
       </c>
       <c r="B38" s="3" t="str">
-        <f t="shared" si="17"/>
-        <v>NA</v>
-      </c>
-      <c r="C38">
-        <v>3</v>
-      </c>
-      <c r="D38">
-        <v>3</v>
-      </c>
-      <c r="E38">
-        <v>3</v>
-      </c>
-      <c r="F38">
-        <v>3</v>
-      </c>
-      <c r="G38">
-        <v>3</v>
-      </c>
-      <c r="H38">
-        <v>3</v>
-      </c>
-      <c r="I38">
-        <v>3</v>
-      </c>
-      <c r="J38">
-        <v>3</v>
-      </c>
-      <c r="K38">
-        <v>3</v>
-      </c>
-      <c r="L38">
-        <v>3</v>
-      </c>
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
       <c r="M38" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
-        <f t="shared" si="16"/>
+        <f>A19</f>
         <v>H</v>
       </c>
       <c r="B39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="C39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="D39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="E39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="F39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="G39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="H39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="I39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="J39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="K39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="L39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="M39" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B41">
         <f>B$1</f>
         <v>1</v>
       </c>
       <c r="C41">
-        <f t="shared" ref="C41:L51" si="18">C$1</f>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="D41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="E41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="F41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="G41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>6</v>
       </c>
       <c r="H41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>7</v>
       </c>
       <c r="I41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="J41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>9</v>
       </c>
       <c r="K41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>10</v>
       </c>
       <c r="L41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>11</v>
       </c>
       <c r="M41">
@@ -2436,7 +2335,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="str">
-        <f t="shared" ref="A42:A49" si="19">A12</f>
+        <f>A22</f>
         <v>A</v>
       </c>
       <c r="B42" s="3" t="str">
@@ -2444,258 +2343,438 @@
         <v>NA</v>
       </c>
       <c r="C42" s="3" t="str">
-        <f t="shared" ref="B42:M49" si="20">$B$2</f>
+        <f t="shared" ref="B42:M49" si="17">$B$2</f>
         <v>NA</v>
       </c>
       <c r="D42" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="E42" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="F42" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="G42" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="H42" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="I42" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="J42" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="K42" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="L42" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="M42" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
-        <f t="shared" si="19"/>
+        <f>A23</f>
         <v>B</v>
       </c>
       <c r="B43" s="3" t="str">
-        <f t="shared" si="20"/>
-        <v>NA</v>
-      </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
+        <f t="shared" si="17"/>
+        <v>NA</v>
+      </c>
+      <c r="C43" s="2" t="e">
+        <f>C33/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D43" s="2" t="e">
+        <f>D33/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E43" s="2" t="e">
+        <f>E33/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F43" s="2" t="e">
+        <f>F33/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G43" s="2" t="e">
+        <f>G33/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H43" s="2" t="e">
+        <f>H33/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I43" s="2" t="e">
+        <f>I33/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J43" s="2" t="e">
+        <f>J33/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K43" s="2" t="e">
+        <f>K33/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L43" s="2" t="e">
+        <f>L33/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="M43" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="str">
-        <f t="shared" si="19"/>
+        <f>A24</f>
         <v>C</v>
       </c>
       <c r="B44" s="3" t="str">
-        <f t="shared" si="20"/>
-        <v>NA</v>
-      </c>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
+        <f t="shared" si="17"/>
+        <v>NA</v>
+      </c>
+      <c r="C44" s="2" t="e">
+        <f>C34/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D44" s="2" t="e">
+        <f>D34/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E44" s="2" t="e">
+        <f>E34/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F44" s="2" t="e">
+        <f>F34/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G44" s="2" t="e">
+        <f>G34/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H44" s="2" t="e">
+        <f>H34/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I44" s="2" t="e">
+        <f>I34/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J44" s="2" t="e">
+        <f>J34/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K44" s="2" t="e">
+        <f>K34/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L44" s="2" t="e">
+        <f>L34/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="M44" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="str">
-        <f t="shared" si="19"/>
+        <f>A25</f>
         <v>D</v>
       </c>
       <c r="B45" s="3" t="str">
-        <f t="shared" si="20"/>
-        <v>NA</v>
-      </c>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
+        <f t="shared" si="17"/>
+        <v>NA</v>
+      </c>
+      <c r="C45" s="2" t="e">
+        <f>C35/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D45" s="2" t="e">
+        <f>D35/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E45" s="2" t="e">
+        <f>E35/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F45" s="2" t="e">
+        <f>F35/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G45" s="2" t="e">
+        <f>G35/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H45" s="2" t="e">
+        <f>H35/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I45" s="2" t="e">
+        <f>I35/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J45" s="2" t="e">
+        <f>J35/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K45" s="2" t="e">
+        <f>K35/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L45" s="2" t="e">
+        <f>L35/AVERAGE($L$33:$L$35)*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="M45" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="str">
-        <f t="shared" si="19"/>
+        <f>A26</f>
         <v>E</v>
       </c>
       <c r="B46" s="3" t="str">
-        <f t="shared" si="20"/>
-        <v>NA</v>
-      </c>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
+        <f t="shared" si="17"/>
+        <v>NA</v>
+      </c>
+      <c r="C46" s="2" t="e">
+        <f>C36/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D46" s="2" t="e">
+        <f>D36/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E46" s="2" t="e">
+        <f>E36/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F46" s="2" t="e">
+        <f>F36/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G46" s="2" t="e">
+        <f>G36/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H46" s="2" t="e">
+        <f>H36/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I46" s="2" t="e">
+        <f>I36/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J46" s="2" t="e">
+        <f>J36/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K46" s="2" t="e">
+        <f>K36/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L46" s="2" t="e">
+        <f>L36/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="M46" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="str">
-        <f t="shared" si="19"/>
+        <f>A27</f>
         <v>F</v>
       </c>
       <c r="B47" s="3" t="str">
-        <f t="shared" si="20"/>
-        <v>NA</v>
-      </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
+        <f t="shared" si="17"/>
+        <v>NA</v>
+      </c>
+      <c r="C47" s="2" t="e">
+        <f>C37/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D47" s="2" t="e">
+        <f>D37/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E47" s="2" t="e">
+        <f>E37/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F47" s="2" t="e">
+        <f>F37/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G47" s="2" t="e">
+        <f>G37/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H47" s="2" t="e">
+        <f>H37/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I47" s="2" t="e">
+        <f>I37/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J47" s="2" t="e">
+        <f>J37/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K47" s="2" t="e">
+        <f>K37/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L47" s="2" t="e">
+        <f>L37/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="M47" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="str">
-        <f t="shared" si="19"/>
+        <f>A28</f>
         <v>G</v>
       </c>
       <c r="B48" s="3" t="str">
-        <f t="shared" si="20"/>
-        <v>NA</v>
-      </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
+        <f t="shared" si="17"/>
+        <v>NA</v>
+      </c>
+      <c r="C48" s="2" t="e">
+        <f>C38/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D48" s="2" t="e">
+        <f>D38/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E48" s="2" t="e">
+        <f>E38/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F48" s="2" t="e">
+        <f>F38/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G48" s="2" t="e">
+        <f>G38/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H48" s="2" t="e">
+        <f>H38/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I48" s="2" t="e">
+        <f>I38/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J48" s="2" t="e">
+        <f>J38/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K48" s="2" t="e">
+        <f>K38/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L48" s="2" t="e">
+        <f>L38/AVERAGE($L$36:$L$38)*100</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="M48" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
-        <f t="shared" si="19"/>
+        <f>A29</f>
         <v>H</v>
       </c>
       <c r="B49" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="C49" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="D49" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="E49" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="F49" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="G49" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="H49" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="I49" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="J49" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="K49" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="L49" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="M49" s="3" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B51">
         <f>B$1</f>
         <v>1</v>
       </c>
       <c r="C51">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="C51:L51" si="18">C$1</f>
         <v>2</v>
       </c>
       <c r="D51">
@@ -2741,7 +2820,7 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="str">
-        <f t="shared" ref="A52:A59" si="21">A22</f>
+        <f>A42</f>
         <v>A</v>
       </c>
       <c r="B52" s="3" t="str">
@@ -2749,425 +2828,365 @@
         <v>NA</v>
       </c>
       <c r="C52" s="3" t="str">
-        <f t="shared" ref="B52:M59" si="22">$B$2</f>
+        <f t="shared" ref="B52:M59" si="19">$B$2</f>
         <v>NA</v>
       </c>
       <c r="D52" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="E52" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="F52" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="G52" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="H52" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="I52" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="J52" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="K52" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="L52" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="M52" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="str">
-        <f t="shared" si="21"/>
+        <f>A43</f>
         <v>B</v>
       </c>
       <c r="B53" s="3" t="str">
-        <f t="shared" si="22"/>
-        <v>NA</v>
-      </c>
-      <c r="C53" s="2" t="e">
-        <f t="shared" ref="C53:K55" si="23">C43/AVERAGE($L$43:$L$45)*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D53" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E53" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F53" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G53" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H53" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I53" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J53" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K53" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L53" s="2" t="e">
-        <f>L43/AVERAGE($L$43:$L$45)*100</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="K53">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>1</v>
       </c>
       <c r="M53" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="str">
-        <f t="shared" si="21"/>
+        <f>A44</f>
         <v>C</v>
       </c>
       <c r="B54" s="3" t="str">
-        <f t="shared" si="22"/>
-        <v>NA</v>
-      </c>
-      <c r="C54" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D54" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E54" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F54" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G54" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H54" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I54" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J54" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K54" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L54" s="2" t="e">
-        <f t="shared" ref="L54:L55" si="24">L44/AVERAGE($L$43:$L$45)*100</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54">
+        <v>2</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+      <c r="H54">
+        <v>2</v>
+      </c>
+      <c r="I54">
+        <v>2</v>
+      </c>
+      <c r="J54">
+        <v>2</v>
+      </c>
+      <c r="K54">
+        <v>2</v>
+      </c>
+      <c r="L54">
+        <v>2</v>
       </c>
       <c r="M54" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="str">
-        <f t="shared" si="21"/>
+        <f>A45</f>
         <v>D</v>
       </c>
       <c r="B55" s="3" t="str">
-        <f t="shared" si="22"/>
-        <v>NA</v>
-      </c>
-      <c r="C55" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D55" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E55" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F55" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G55" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H55" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I55" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J55" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K55" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L55" s="2" t="e">
-        <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55">
+        <v>3</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+      <c r="F55">
+        <v>3</v>
+      </c>
+      <c r="G55">
+        <v>3</v>
+      </c>
+      <c r="H55">
+        <v>3</v>
+      </c>
+      <c r="I55">
+        <v>3</v>
+      </c>
+      <c r="J55">
+        <v>3</v>
+      </c>
+      <c r="K55">
+        <v>3</v>
+      </c>
+      <c r="L55">
+        <v>3</v>
       </c>
       <c r="M55" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="str">
-        <f t="shared" si="21"/>
+        <f>A46</f>
         <v>E</v>
       </c>
       <c r="B56" s="3" t="str">
-        <f t="shared" si="22"/>
-        <v>NA</v>
-      </c>
-      <c r="C56" s="2" t="e">
-        <f t="shared" ref="C56:K58" si="25">C46/AVERAGE($L$46:$L$48)*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D56" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E56" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F56" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G56" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H56" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I56" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J56" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K56" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L56" s="2" t="e">
-        <f>L46/AVERAGE($L$46:$L$48)*100</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="K56">
+        <v>1</v>
+      </c>
+      <c r="L56">
+        <v>1</v>
       </c>
       <c r="M56" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="str">
-        <f t="shared" si="21"/>
+        <f>A47</f>
         <v>F</v>
       </c>
       <c r="B57" s="3" t="str">
-        <f t="shared" si="22"/>
-        <v>NA</v>
-      </c>
-      <c r="C57" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D57" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E57" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F57" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G57" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H57" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I57" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J57" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K57" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L57" s="2" t="e">
-        <f t="shared" ref="L57:L58" si="26">L47/AVERAGE($L$46:$L$48)*100</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57">
+        <v>2</v>
+      </c>
+      <c r="G57">
+        <v>2</v>
+      </c>
+      <c r="H57">
+        <v>2</v>
+      </c>
+      <c r="I57">
+        <v>2</v>
+      </c>
+      <c r="J57">
+        <v>2</v>
+      </c>
+      <c r="K57">
+        <v>2</v>
+      </c>
+      <c r="L57">
+        <v>2</v>
       </c>
       <c r="M57" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="str">
-        <f t="shared" si="21"/>
+        <f>A48</f>
         <v>G</v>
       </c>
       <c r="B58" s="3" t="str">
-        <f t="shared" si="22"/>
-        <v>NA</v>
-      </c>
-      <c r="C58" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D58" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E58" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F58" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G58" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H58" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I58" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J58" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K58" s="2" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L58" s="2" t="e">
-        <f t="shared" si="26"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+      <c r="D58">
+        <v>3</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="F58">
+        <v>3</v>
+      </c>
+      <c r="G58">
+        <v>3</v>
+      </c>
+      <c r="H58">
+        <v>3</v>
+      </c>
+      <c r="I58">
+        <v>3</v>
+      </c>
+      <c r="J58">
+        <v>3</v>
+      </c>
+      <c r="K58">
+        <v>3</v>
+      </c>
+      <c r="L58">
+        <v>3</v>
       </c>
       <c r="M58" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="str">
-        <f t="shared" si="21"/>
+        <f>A49</f>
         <v>H</v>
       </c>
       <c r="B59" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="C59" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="D59" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="E59" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="F59" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="G59" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="H59" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="I59" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="J59" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="K59" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="L59" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="M59" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last commit didn't seem to capture many changes to script, for some reason. same changes, better comments. also updating example import files and plate template
</commit_message>
<xml_diff>
--- a/JWS CTG plater import template.xlsx
+++ b/JWS CTG plater import template.xlsx
@@ -6,10 +6,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevenson/Library/CloudStorage/Box-Box/Shokat/bio lab notebook/JS-B2-79 CTG K562 DasatiLink PonatiLink/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevenson/Documents/git/plateplotr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B9E927-EDF7-AA41-9AB3-C8E09F772BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69323F3-DC5E-984B-BFFB-A86E3207E31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{2712D622-CD40-B842-AED5-08F459FD295F}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
-    <t>drug</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -59,12 +56,6 @@
     <t>G</t>
   </si>
   <si>
-    <t>concentration</t>
-  </si>
-  <si>
-    <t>CTG</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -72,9 +63,6 @@
   </si>
   <si>
     <t>replicate</t>
-  </si>
-  <si>
-    <t>CTG_normalized</t>
   </si>
   <si>
     <t>cell_line</t>
@@ -92,7 +80,19 @@
     <t>initial conc (uM)</t>
   </si>
   <si>
-    <t>drug name</t>
+    <t>compound</t>
+  </si>
+  <si>
+    <t>compound name</t>
+  </si>
+  <si>
+    <t>readout</t>
+  </si>
+  <si>
+    <t>read_norm</t>
+  </si>
+  <si>
+    <t>conc</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -548,7 +548,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -589,10 +589,10 @@
     </row>
     <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="str">
         <f>$B$2</f>
@@ -641,50 +641,50 @@
     </row>
     <row r="3" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="3" t="str">
         <f t="shared" ref="B3:B8" si="1">$B$2</f>
         <v>NA</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:L8" si="2">$C$3</f>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="M3" s="3" t="str">
         <f t="shared" ref="M3:M9" si="3">$B$2</f>
@@ -693,7 +693,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="3" t="str">
         <f t="shared" si="1"/>
@@ -701,43 +701,43 @@
       </c>
       <c r="C4" t="str">
         <f>$C$3</f>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="M4" s="3" t="str">
         <f t="shared" si="3"/>
@@ -746,7 +746,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="str">
         <f t="shared" si="1"/>
@@ -754,43 +754,43 @@
       </c>
       <c r="C5" t="str">
         <f>$C$3</f>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="M5" s="3" t="str">
         <f t="shared" si="3"/>
@@ -799,7 +799,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="3" t="str">
         <f t="shared" si="1"/>
@@ -807,43 +807,43 @@
       </c>
       <c r="C6" t="str">
         <f>$C$3</f>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="M6" s="3" t="str">
         <f t="shared" si="3"/>
@@ -852,7 +852,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="3" t="str">
         <f t="shared" si="1"/>
@@ -860,43 +860,43 @@
       </c>
       <c r="C7" t="str">
         <f>$C$3</f>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="M7" s="3" t="str">
         <f t="shared" si="3"/>
@@ -905,7 +905,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3" t="str">
         <f t="shared" si="1"/>
@@ -913,43 +913,43 @@
       </c>
       <c r="C8" t="str">
         <f>$C$3</f>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="2"/>
-        <v>drug name</v>
+        <v>compound name</v>
       </c>
       <c r="M8" s="3" t="str">
         <f t="shared" si="3"/>
@@ -958,7 +958,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3" t="str">
         <f t="shared" ref="B9:L9" si="4">$B$2</f>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <f>B$1</f>
@@ -1126,7 +1126,7 @@
         <v>NA</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D13" s="2" t="e">
         <f>C13/3</f>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B21">
         <f>B$1</f>
@@ -1609,7 +1609,7 @@
         <v>NA</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" ref="D23:L25" si="13">$C$23</f>
@@ -1770,7 +1770,7 @@
         <v>NA</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" ref="D26:L28" si="14">$C$26</f>
@@ -1977,7 +1977,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B31">
         <f>B$1</f>
@@ -2030,7 +2030,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
-        <f>A12</f>
+        <f t="shared" ref="A32:A39" si="16">A12</f>
         <v>A</v>
       </c>
       <c r="B32" s="3" t="str">
@@ -2038,57 +2038,57 @@
         <v>NA</v>
       </c>
       <c r="C32" s="3" t="str">
-        <f t="shared" ref="B32:M39" si="16">$B$2</f>
+        <f t="shared" ref="B32:M39" si="17">$B$2</f>
         <v>NA</v>
       </c>
       <c r="D32" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="E32" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="F32" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="G32" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="H32" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="I32" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="J32" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="K32" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="L32" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="M32" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
-        <f>A13</f>
+        <f t="shared" si="16"/>
         <v>B</v>
       </c>
       <c r="B33" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="C33" s="1"/>
@@ -2102,17 +2102,17 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
-        <f>A14</f>
+        <f t="shared" si="16"/>
         <v>C</v>
       </c>
       <c r="B34" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="C34" s="1"/>
@@ -2126,17 +2126,17 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
-        <f>A15</f>
+        <f t="shared" si="16"/>
         <v>D</v>
       </c>
       <c r="B35" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="C35" s="1"/>
@@ -2150,17 +2150,17 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
-        <f>A16</f>
+        <f t="shared" si="16"/>
         <v>E</v>
       </c>
       <c r="B36" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="C36" s="1"/>
@@ -2174,17 +2174,17 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
-        <f>A17</f>
+        <f t="shared" si="16"/>
         <v>F</v>
       </c>
       <c r="B37" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="C37" s="1"/>
@@ -2198,17 +2198,17 @@
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
-        <f>A18</f>
+        <f t="shared" si="16"/>
         <v>G</v>
       </c>
       <c r="B38" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="C38" s="1"/>
@@ -2222,67 +2222,67 @@
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
-        <f>A19</f>
+        <f t="shared" si="16"/>
         <v>H</v>
       </c>
       <c r="B39" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="C39" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="D39" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="E39" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="F39" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="G39" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="H39" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="I39" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="J39" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="K39" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="L39" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="M39" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B41">
         <f>B$1</f>
@@ -2335,7 +2335,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="str">
-        <f>A22</f>
+        <f t="shared" ref="A42:A49" si="18">A22</f>
         <v>A</v>
       </c>
       <c r="B42" s="3" t="str">
@@ -2343,474 +2343,474 @@
         <v>NA</v>
       </c>
       <c r="C42" s="3" t="str">
-        <f t="shared" ref="B42:M49" si="17">$B$2</f>
+        <f t="shared" ref="B42:M49" si="19">$B$2</f>
         <v>NA</v>
       </c>
       <c r="D42" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="E42" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="F42" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="G42" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="H42" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="I42" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="J42" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="K42" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="L42" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="M42" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
-        <f>A23</f>
+        <f t="shared" si="18"/>
         <v>B</v>
       </c>
       <c r="B43" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="C43" s="2" t="e">
-        <f>C33/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" ref="C43:L43" si="20">C33/AVERAGE($L$33:$L$35)*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D43" s="2" t="e">
-        <f>D33/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E43" s="2" t="e">
-        <f>E33/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F43" s="2" t="e">
-        <f>F33/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G43" s="2" t="e">
-        <f>G33/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H43" s="2" t="e">
-        <f>H33/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I43" s="2" t="e">
-        <f>I33/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J43" s="2" t="e">
-        <f>J33/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K43" s="2" t="e">
-        <f>K33/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L43" s="2" t="e">
-        <f>L33/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M43" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="str">
-        <f>A24</f>
+        <f t="shared" si="18"/>
         <v>C</v>
       </c>
       <c r="B44" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="C44" s="2" t="e">
-        <f>C34/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" ref="C44:L44" si="21">C34/AVERAGE($L$33:$L$35)*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D44" s="2" t="e">
-        <f>D34/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E44" s="2" t="e">
-        <f>E34/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F44" s="2" t="e">
-        <f>F34/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G44" s="2" t="e">
-        <f>G34/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H44" s="2" t="e">
-        <f>H34/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I44" s="2" t="e">
-        <f>I34/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J44" s="2" t="e">
-        <f>J34/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K44" s="2" t="e">
-        <f>K34/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L44" s="2" t="e">
-        <f>L34/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M44" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="str">
-        <f>A25</f>
+        <f t="shared" si="18"/>
         <v>D</v>
       </c>
       <c r="B45" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="C45" s="2" t="e">
-        <f>C35/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" ref="C45:L45" si="22">C35/AVERAGE($L$33:$L$35)*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D45" s="2" t="e">
-        <f>D35/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E45" s="2" t="e">
-        <f>E35/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F45" s="2" t="e">
-        <f>F35/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G45" s="2" t="e">
-        <f>G35/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H45" s="2" t="e">
-        <f>H35/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I45" s="2" t="e">
-        <f>I35/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J45" s="2" t="e">
-        <f>J35/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K45" s="2" t="e">
-        <f>K35/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L45" s="2" t="e">
-        <f>L35/AVERAGE($L$33:$L$35)*100</f>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M45" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="str">
-        <f>A26</f>
+        <f t="shared" si="18"/>
         <v>E</v>
       </c>
       <c r="B46" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="C46" s="2" t="e">
-        <f>C36/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" ref="C46:L46" si="23">C36/AVERAGE($L$36:$L$38)*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D46" s="2" t="e">
-        <f>D36/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E46" s="2" t="e">
-        <f>E36/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F46" s="2" t="e">
-        <f>F36/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G46" s="2" t="e">
-        <f>G36/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H46" s="2" t="e">
-        <f>H36/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I46" s="2" t="e">
-        <f>I36/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J46" s="2" t="e">
-        <f>J36/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K46" s="2" t="e">
-        <f>K36/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L46" s="2" t="e">
-        <f>L36/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M46" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="str">
-        <f>A27</f>
+        <f t="shared" si="18"/>
         <v>F</v>
       </c>
       <c r="B47" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="C47" s="2" t="e">
-        <f>C37/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" ref="C47:L47" si="24">C37/AVERAGE($L$36:$L$38)*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D47" s="2" t="e">
-        <f>D37/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E47" s="2" t="e">
-        <f>E37/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F47" s="2" t="e">
-        <f>F37/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G47" s="2" t="e">
-        <f>G37/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H47" s="2" t="e">
-        <f>H37/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I47" s="2" t="e">
-        <f>I37/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J47" s="2" t="e">
-        <f>J37/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K47" s="2" t="e">
-        <f>K37/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L47" s="2" t="e">
-        <f>L37/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M47" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="str">
-        <f>A28</f>
+        <f t="shared" si="18"/>
         <v>G</v>
       </c>
       <c r="B48" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="C48" s="2" t="e">
-        <f>C38/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" ref="C48:L48" si="25">C38/AVERAGE($L$36:$L$38)*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D48" s="2" t="e">
-        <f>D38/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E48" s="2" t="e">
-        <f>E38/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F48" s="2" t="e">
-        <f>F38/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G48" s="2" t="e">
-        <f>G38/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H48" s="2" t="e">
-        <f>H38/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I48" s="2" t="e">
-        <f>I38/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J48" s="2" t="e">
-        <f>J38/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K48" s="2" t="e">
-        <f>K38/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L48" s="2" t="e">
-        <f>L38/AVERAGE($L$36:$L$38)*100</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M48" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
-        <f>A29</f>
+        <f t="shared" si="18"/>
         <v>H</v>
       </c>
       <c r="B49" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="C49" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="D49" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="E49" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="F49" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="G49" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="H49" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="I49" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="J49" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="K49" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="L49" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="M49" s="3" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B51">
         <f>B$1</f>
         <v>1</v>
       </c>
       <c r="C51">
-        <f t="shared" ref="C51:L51" si="18">C$1</f>
+        <f t="shared" ref="C51:L51" si="26">C$1</f>
         <v>2</v>
       </c>
       <c r="D51">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>3</v>
       </c>
       <c r="E51">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>4</v>
       </c>
       <c r="F51">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>5</v>
       </c>
       <c r="G51">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>6</v>
       </c>
       <c r="H51">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>7</v>
       </c>
       <c r="I51">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>8</v>
       </c>
       <c r="J51">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>9</v>
       </c>
       <c r="K51">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="L51">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>11</v>
       </c>
       <c r="M51">
@@ -2820,7 +2820,7 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="str">
-        <f>A42</f>
+        <f t="shared" ref="A52:A59" si="27">A42</f>
         <v>A</v>
       </c>
       <c r="B52" s="3" t="str">
@@ -2828,57 +2828,57 @@
         <v>NA</v>
       </c>
       <c r="C52" s="3" t="str">
-        <f t="shared" ref="B52:M59" si="19">$B$2</f>
+        <f t="shared" ref="B52:M59" si="28">$B$2</f>
         <v>NA</v>
       </c>
       <c r="D52" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="E52" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="F52" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="G52" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="H52" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="I52" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="J52" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="K52" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="L52" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="M52" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="str">
-        <f>A43</f>
+        <f t="shared" si="27"/>
         <v>B</v>
       </c>
       <c r="B53" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="C53">
@@ -2912,17 +2912,17 @@
         <v>1</v>
       </c>
       <c r="M53" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="str">
-        <f>A44</f>
+        <f t="shared" si="27"/>
         <v>C</v>
       </c>
       <c r="B54" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="C54">
@@ -2956,17 +2956,17 @@
         <v>2</v>
       </c>
       <c r="M54" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="str">
-        <f>A45</f>
+        <f t="shared" si="27"/>
         <v>D</v>
       </c>
       <c r="B55" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="C55">
@@ -3000,17 +3000,17 @@
         <v>3</v>
       </c>
       <c r="M55" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="str">
-        <f>A46</f>
+        <f t="shared" si="27"/>
         <v>E</v>
       </c>
       <c r="B56" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="C56">
@@ -3044,17 +3044,17 @@
         <v>1</v>
       </c>
       <c r="M56" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="str">
-        <f>A47</f>
+        <f t="shared" si="27"/>
         <v>F</v>
       </c>
       <c r="B57" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="C57">
@@ -3088,17 +3088,17 @@
         <v>2</v>
       </c>
       <c r="M57" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="str">
-        <f>A48</f>
+        <f t="shared" si="27"/>
         <v>G</v>
       </c>
       <c r="B58" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="C58">
@@ -3132,61 +3132,61 @@
         <v>3</v>
       </c>
       <c r="M58" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="str">
-        <f>A49</f>
+        <f t="shared" si="27"/>
         <v>H</v>
       </c>
       <c r="B59" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="C59" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="D59" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="E59" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="F59" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="G59" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="H59" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="I59" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="J59" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="K59" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="L59" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
       <c r="M59" s="3" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed conc to conc_uM
</commit_message>
<xml_diff>
--- a/JWS CTG plater import template.xlsx
+++ b/JWS CTG plater import template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevenson/Documents/git/plateplotr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69323F3-DC5E-984B-BFFB-A86E3207E31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFE4567-0DDE-3D4A-B105-42016946D5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{2712D622-CD40-B842-AED5-08F459FD295F}"/>
   </bookViews>
@@ -92,7 +92,7 @@
     <t>read_norm</t>
   </si>
   <si>
-    <t>conc</t>
+    <t>conc_uM</t>
   </si>
 </sst>
 </file>

</xml_diff>